<commit_message>
edited to fix test_RRTs.py which had an issue with data types conversion
</commit_message>
<xml_diff>
--- a/tests/sample_file.xlsx
+++ b/tests/sample_file.xlsx
@@ -441,65 +441,65 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Retention Time</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Area</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Retention Time</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>1:A,1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>1:A,1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>1:B,1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>1:B,1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>